<commit_message>
cases-de.xlsx: When will it be 1 Mill cases
</commit_message>
<xml_diff>
--- a/data/cases-de.xlsx
+++ b/data/cases-de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torben/Hacken/GitHub/COVID-19-Coronavirus-German-Regions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EFC311-E885-074D-96C9-057B950B3D30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD0167B-4294-954D-B436-E257A5F4FB0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{309167EE-B9E7-9F44-B3F3-07C1908B9528}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" activeTab="8" xr2:uid="{309167EE-B9E7-9F44-B3F3-07C1908B9528}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="10" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Cases Change" sheetId="11" r:id="rId6"/>
     <sheet name="Death" sheetId="5" r:id="rId7"/>
     <sheet name="RefPopulation" sheetId="12" r:id="rId8"/>
+    <sheet name="When will it be 1 Mill cases" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="71">
   <si>
     <t>Baden-Württemberg</t>
   </si>
@@ -243,6 +244,21 @@
   </si>
   <si>
     <t>world data at GitHub</t>
+  </si>
+  <si>
+    <t>Cases today</t>
+  </si>
+  <si>
+    <t>Duplications</t>
+  </si>
+  <si>
+    <t>Number to reach</t>
+  </si>
+  <si>
+    <t>Duplication time today</t>
+  </si>
+  <si>
+    <t>Days</t>
   </si>
 </sst>
 </file>
@@ -4434,7 +4450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05B1DF0-9508-684D-9C94-CA87D158EEEF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -7080,8 +7096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233E67D7-4FF2-D745-A107-DDC4CB6E1273}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10042,7 +10058,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10220,4 +10236,61 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD699B48-9B9A-DD49-8864-472A6998CAC7}">
+  <dimension ref="A2:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>2369</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="22">
+        <f xml:space="preserve"> LOG(B3/B2,2)</f>
+        <v>8.7215060860839433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="52">
+        <f>B4*E2</f>
+        <v>26.164518258251832</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gnuplot plots in DE and added Anstiegsfaktor
</commit_message>
<xml_diff>
--- a/data/cases-de.xlsx
+++ b/data/cases-de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torben/Hacken/GitHub/COVID-19-Coronavirus-German-Regions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF4D45-4000-8040-AAAC-27518B4F4C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28BBABB-9E59-C94E-B283-0B250D78F867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14320" firstSheet="1" activeTab="6" xr2:uid="{309167EE-B9E7-9F44-B3F3-07C1908B9528}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14320" firstSheet="3" activeTab="9" xr2:uid="{309167EE-B9E7-9F44-B3F3-07C1908B9528}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="10" r:id="rId1"/>
@@ -404,7 +404,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -813,7 +813,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6275,7 +6275,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -6523,6 +6523,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="188829200"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -8314,7 +8315,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>564250</xdr:colOff>
+      <xdr:colOff>272150</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>338550</xdr:rowOff>
     </xdr:to>
@@ -8919,8 +8920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD699B48-9B9A-DD49-8864-472A6998CAC7}">
   <dimension ref="A2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12114,8 +12115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233E67D7-4FF2-D745-A107-DDC4CB6E1273}">
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
@@ -14947,8 +14948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C283F65E-4645-8A47-BFE2-5D2317004015}">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>